<commit_message>
Correctif recap valdiateur,Ajout règle gestion
Correctif recap valdiateur,Ajout règle gestion pour vérifier la présence de data sans rendre obligatoire pour ne pas l'afficher lors de _elements
</commit_message>
<xml_diff>
--- a/input/images/20230706_Prod_ESMS_RecapValidateurs.xlsx
+++ b/input/images/20230706_Prod_ESMS_RecapValidateurs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Réalisation\Conseil\ASIP\ANS-006 Contrat cadre CI SIS 2021\Projets\ANS-006-84_SDO_ESMS_TDD_MAJ\4_Production\SDO_ESMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tru\Documents\GitHub\IG-fhir-medicosocial-suivi-decisions-orientation\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34F6D7F-7E2F-4BD7-AE24-8739A798380E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0EA216-D9ED-461D-817F-6104DC530717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18450" yWindow="0" windowWidth="18420" windowHeight="17385" xr2:uid="{CAB0CB30-A5BF-4132-AD82-A1FC13727143}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAB0CB30-A5BF-4132-AD82-A1FC13727143}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>Ressource testée</t>
   </si>
@@ -172,18 +172,12 @@
     <t>SDOTask_nonPassant.json</t>
   </si>
   <si>
-    <t>https://example.com/base/DocumentReference?id=test</t>
-  </si>
-  <si>
     <t>ESMSConsent_nonPassant.json</t>
   </si>
   <si>
     <t>https://example.com/base/DocumentReference?identifier=idNat_decision</t>
   </si>
   <si>
-    <t>https://example.com/base/Task?id=test</t>
-  </si>
-  <si>
     <t>Validateur d'URL</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
     <t>SDOBundleResultatRechercheNotificationESMS_nonPassant.json</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/EVSClient/detailedResult.seam?type=FHIR&amp;oid=1.3.6.1.4.1.12559.11.36.3.1.70291</t>
-  </si>
-  <si>
     <t>https://interop.esante.gouv.fr/EVSClient/detailedResult.seam?type=FHIR&amp;oid=1.3.6.1.4.1.12559.11.36.3.1.70292</t>
   </si>
   <si>
@@ -238,9 +229,6 @@
     <t>https://interop.esante.gouv.fr/EVSClient/detailedResult.seam?type=FHIR&amp;oid=1.3.6.1.4.1.12559.11.36.3.1.70302</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/EVSClient/detailedResult.seam?type=FHIR&amp;oid=1.3.6.1.4.1.12559.11.36.3.1.70306</t>
-  </si>
-  <si>
     <t>https://interop.esante.gouv.fr/EVSClient/detailedResult.seam?type=FHIR&amp;oid=1.3.6.1.4.1.12559.11.36.3.1.70307</t>
   </si>
   <si>
@@ -311,6 +299,12 @@
   </si>
   <si>
     <t>https://interop.esante.gouv.fr/evs/report.seam?oid=1.3.6.1.4.1.12559.11.36.4.15655</t>
+  </si>
+  <si>
+    <t>https://example.com/base/DocumentReference/test</t>
+  </si>
+  <si>
+    <t>https://example.com/base/Task/test</t>
   </si>
 </sst>
 </file>
@@ -756,7 +750,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -863,6 +857,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1180,49 +1176,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3196A800-90B5-4CE1-A4D6-14B5DEF4AE04}">
   <dimension ref="B1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="82" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" customWidth="1"/>
+    <col min="3" max="3" width="57.1796875" customWidth="1"/>
+    <col min="4" max="4" width="55.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="56" customWidth="1"/>
-    <col min="8" max="8" width="51.28515625" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.26953125" customWidth="1"/>
+    <col min="9" max="9" width="55.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="52" t="s">
         <v>15</v>
       </c>
@@ -1244,7 +1240,7 @@
       </c>
       <c r="I6" s="51"/>
     </row>
-    <row r="7" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="53"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
@@ -1262,7 +1258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
         <v>3</v>
       </c>
@@ -1277,24 +1273,24 @@
         <v>34</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H8" s="31" t="s">
         <v>38</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>21</v>
@@ -1303,22 +1299,22 @@
         <v>24</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="36" t="s">
         <v>3</v>
       </c>
@@ -1329,28 +1325,26 @@
       <c r="E10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="F10" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="9"/>
       <c r="H10" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>20</v>
@@ -1362,19 +1356,19 @@
         <v>26</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="39" t="s">
         <v>14</v>
       </c>
@@ -1388,27 +1382,27 @@
         <v>7</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I12" s="49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>32</v>
@@ -1420,19 +1414,19 @@
         <v>25</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="40" t="s">
         <v>3</v>
       </c>
@@ -1447,19 +1441,19 @@
         <v>16</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="39" t="s">
         <v>14</v>
       </c>
@@ -1473,51 +1467,51 @@
         <v>40</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I15" s="49" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>44</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="40" t="s">
         <v>3</v>
       </c>
@@ -1532,24 +1526,24 @@
         <v>13</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>29</v>
@@ -1561,19 +1555,19 @@
         <v>33</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="41" t="s">
         <v>3</v>
       </c>
@@ -1584,23 +1578,21 @@
       <c r="E19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>61</v>
-      </c>
+      <c r="F19" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="46"/>
       <c r="H19" s="45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H20" s="2"/>
     </row>
   </sheetData>
@@ -1622,34 +1614,32 @@
     <hyperlink ref="H14" r:id="rId6" xr:uid="{0A421C85-E220-4F2D-925A-D06E8B861987}"/>
     <hyperlink ref="H19" r:id="rId7" xr:uid="{51C658BD-58B2-4DBF-8ABB-52055DB0F332}"/>
     <hyperlink ref="F19" r:id="rId8" xr:uid="{4D81A8B0-CB05-4053-8EC5-D79DFAE041C5}"/>
-    <hyperlink ref="G19" r:id="rId9" xr:uid="{106BFEA4-F0F6-423F-84EE-3D246C85BD0F}"/>
-    <hyperlink ref="I19" r:id="rId10" xr:uid="{5FC67934-0EFB-4978-9708-E181ED4ACE84}"/>
-    <hyperlink ref="F17" r:id="rId11" xr:uid="{81ADB453-8AA3-4328-8DBF-A74F0B52C0AD}"/>
-    <hyperlink ref="H17" r:id="rId12" xr:uid="{139394CC-675B-4378-B07C-75EDE295F744}"/>
-    <hyperlink ref="G17" r:id="rId13" xr:uid="{F23EF613-F40F-4D54-8474-A967625F6EBD}"/>
-    <hyperlink ref="I17" r:id="rId14" xr:uid="{09B5BED0-1E7C-4193-8999-F2803D75BAA7}"/>
-    <hyperlink ref="G8" r:id="rId15" xr:uid="{DC961034-EBB3-4797-A55C-35072AABDEC5}"/>
-    <hyperlink ref="I8" r:id="rId16" xr:uid="{7D223A23-F7CD-470B-84B3-1ADDB991FAB5}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{301B04F4-FD4F-4930-B43A-FB8C345D2E7B}"/>
-    <hyperlink ref="I10" r:id="rId18" xr:uid="{5A04A72E-D35D-4E11-8081-7759E82ED20B}"/>
-    <hyperlink ref="G14" r:id="rId19" xr:uid="{9E6F6BA2-C1F8-422C-AA16-4D689A39AEEF}"/>
-    <hyperlink ref="I14" r:id="rId20" xr:uid="{4BBDFE3C-CFA4-4E1F-A0ED-F4DD2513F781}"/>
-    <hyperlink ref="G12" r:id="rId21" xr:uid="{2DCE75C8-A571-47E2-BE9E-FC95712FC017}"/>
-    <hyperlink ref="I12" r:id="rId22" xr:uid="{4D9B47AE-6CFE-45D1-B0FC-36546799E2B0}"/>
-    <hyperlink ref="G15" r:id="rId23" xr:uid="{8D6E53A1-AEB3-4191-A228-6D338A682695}"/>
-    <hyperlink ref="I15" r:id="rId24" xr:uid="{1B4035E9-5F71-4707-8D1F-336BBC3B34CE}"/>
-    <hyperlink ref="G9" r:id="rId25" xr:uid="{F6C9A908-4792-4E08-B644-5F599570E21D}"/>
-    <hyperlink ref="I9" r:id="rId26" xr:uid="{437FBF8C-E2C6-4BA9-8024-BBBEF9B726F0}"/>
-    <hyperlink ref="G13" r:id="rId27" xr:uid="{000F7A3B-EE56-4FC6-9776-9D348F13EEEF}"/>
-    <hyperlink ref="I13" r:id="rId28" xr:uid="{CA999F75-38B8-41F9-AAEF-E08ED74610DE}"/>
-    <hyperlink ref="G11" r:id="rId29" xr:uid="{C66ABF41-320F-4153-9557-C5A52A8396EB}"/>
-    <hyperlink ref="I11" r:id="rId30" xr:uid="{3EEAA4D6-5326-4C9E-B7A1-452290C61047}"/>
-    <hyperlink ref="G18" r:id="rId31" xr:uid="{8033B8EA-12D3-4708-BE7D-0915239494CC}"/>
-    <hyperlink ref="I18" r:id="rId32" xr:uid="{1CF1879C-4CE2-4092-B8CC-106B2F578E84}"/>
-    <hyperlink ref="G16" r:id="rId33" xr:uid="{5DBE8E42-2D78-4ADC-A399-B57D5B5DEF3D}"/>
-    <hyperlink ref="I16" r:id="rId34" xr:uid="{D66FE8D9-A8F8-4439-93A0-F26A952E7109}"/>
+    <hyperlink ref="I19" r:id="rId9" xr:uid="{5FC67934-0EFB-4978-9708-E181ED4ACE84}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{81ADB453-8AA3-4328-8DBF-A74F0B52C0AD}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{139394CC-675B-4378-B07C-75EDE295F744}"/>
+    <hyperlink ref="G17" r:id="rId12" xr:uid="{F23EF613-F40F-4D54-8474-A967625F6EBD}"/>
+    <hyperlink ref="I17" r:id="rId13" xr:uid="{09B5BED0-1E7C-4193-8999-F2803D75BAA7}"/>
+    <hyperlink ref="G8" r:id="rId14" xr:uid="{DC961034-EBB3-4797-A55C-35072AABDEC5}"/>
+    <hyperlink ref="I8" r:id="rId15" xr:uid="{7D223A23-F7CD-470B-84B3-1ADDB991FAB5}"/>
+    <hyperlink ref="I10" r:id="rId16" xr:uid="{5A04A72E-D35D-4E11-8081-7759E82ED20B}"/>
+    <hyperlink ref="G14" r:id="rId17" xr:uid="{9E6F6BA2-C1F8-422C-AA16-4D689A39AEEF}"/>
+    <hyperlink ref="I14" r:id="rId18" xr:uid="{4BBDFE3C-CFA4-4E1F-A0ED-F4DD2513F781}"/>
+    <hyperlink ref="G12" r:id="rId19" xr:uid="{2DCE75C8-A571-47E2-BE9E-FC95712FC017}"/>
+    <hyperlink ref="I12" r:id="rId20" xr:uid="{4D9B47AE-6CFE-45D1-B0FC-36546799E2B0}"/>
+    <hyperlink ref="G15" r:id="rId21" xr:uid="{8D6E53A1-AEB3-4191-A228-6D338A682695}"/>
+    <hyperlink ref="I15" r:id="rId22" xr:uid="{1B4035E9-5F71-4707-8D1F-336BBC3B34CE}"/>
+    <hyperlink ref="G9" r:id="rId23" xr:uid="{F6C9A908-4792-4E08-B644-5F599570E21D}"/>
+    <hyperlink ref="I9" r:id="rId24" xr:uid="{437FBF8C-E2C6-4BA9-8024-BBBEF9B726F0}"/>
+    <hyperlink ref="G13" r:id="rId25" xr:uid="{000F7A3B-EE56-4FC6-9776-9D348F13EEEF}"/>
+    <hyperlink ref="I13" r:id="rId26" xr:uid="{CA999F75-38B8-41F9-AAEF-E08ED74610DE}"/>
+    <hyperlink ref="G11" r:id="rId27" xr:uid="{C66ABF41-320F-4153-9557-C5A52A8396EB}"/>
+    <hyperlink ref="I11" r:id="rId28" xr:uid="{3EEAA4D6-5326-4C9E-B7A1-452290C61047}"/>
+    <hyperlink ref="G18" r:id="rId29" xr:uid="{8033B8EA-12D3-4708-BE7D-0915239494CC}"/>
+    <hyperlink ref="I18" r:id="rId30" xr:uid="{1CF1879C-4CE2-4092-B8CC-106B2F578E84}"/>
+    <hyperlink ref="G16" r:id="rId31" xr:uid="{5DBE8E42-2D78-4ADC-A399-B57D5B5DEF3D}"/>
+    <hyperlink ref="I16" r:id="rId32" xr:uid="{D66FE8D9-A8F8-4439-93A0-F26A952E7109}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>